<commit_message>
Updated test script and matrix.  crcN works with some test cases and shows bugs for others
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8060"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Short Form Testing" sheetId="3" r:id="rId1"/>
+    <sheet name="Long Form Testing" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>CRC Length</t>
   </si>
@@ -93,6 +94,21 @@
   </si>
   <si>
     <t>7C769F</t>
+  </si>
+  <si>
+    <t>6E1F</t>
+  </si>
+  <si>
+    <t>B59E</t>
+  </si>
+  <si>
+    <t>25CD</t>
+  </si>
+  <si>
+    <t>69F</t>
+  </si>
+  <si>
+    <t>1011010111000</t>
   </si>
 </sst>
 </file>
@@ -108,12 +124,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -138,6 +166,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,9 +454,488 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="8.1796875" customWidth="1"/>
+    <col min="5" max="5" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.90625" customWidth="1"/>
+    <col min="12" max="12" width="21.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1011</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2">
+        <v>101</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7">
+        <v>10011</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="2">
+        <v>1110</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <v>1001</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
+        <v>1111</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7">
+        <v>100101</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <v>11000</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
+        <v>10101</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1100111</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="2">
+        <v>1011</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>110</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
+        <v>111</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2">
+        <v>10011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7">
+        <v>11001011</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2">
+        <v>11011</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>1001110</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
+        <v>11101</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2">
+        <v>1011000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7">
+        <v>111001111</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="2">
+        <v>10111100</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
+        <v>10101110</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
+        <v>11111110</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2">
+        <v>10101110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1000110011</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2">
+        <v>1001010</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>11</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2">
+        <v>101111001</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2">
+        <v>101000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7">
+        <v>11001001111</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="2">
+        <v>1110011000</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
+        <v>101010100</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2">
+        <v>111101001</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2">
+        <v>1101110000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7">
+        <v>101110110111</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="2">
+        <v>101101000</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
+        <v>1000010000</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2">
+        <v>11011111111</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2">
+        <v>11011010000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1001100001111</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="2">
+        <v>111011101011</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2">
+        <v>1010110100</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2">
+        <v>111000001000</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2">
+        <v>100001100111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7">
+        <v>11010101111111</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6">
+        <v>11110001010</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="2">
+        <v>1101010100101</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7">
+        <v>100111110011111</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="2">
+        <v>111101001000</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="8">
+        <v>11001010100100</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8">
+        <v>1000110011</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
+        <v>100111100</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1000111</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2">
+        <v>110010010</v>
+      </c>
+      <c r="G15" s="2">
+        <v>100111</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1010110</v>
+      </c>
+      <c r="I15" s="8">
+        <v>10001</v>
+      </c>
+      <c r="J15" s="8">
+        <v>1101001101110</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1">
+        <v>10001101100</v>
+      </c>
+      <c r="D16" s="1">
+        <v>101011</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2">
+        <v>1111001100</v>
+      </c>
+      <c r="G16" s="2">
+        <v>10110</v>
+      </c>
+      <c r="H16" s="2">
+        <v>10010010</v>
+      </c>
+      <c r="I16" s="2">
+        <v>11111011</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1110011010</v>
+      </c>
+      <c r="K16" s="2">
+        <v>110101</v>
+      </c>
+      <c r="L16" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="E3:E16"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
crcN fully functional, removed unneeded input and cleaned up comments
In addition the max crc length for a two-byte integer was set to 15.
This is because a 16-bit crc has a polynomial of length of 17 which is
larger than the data it is operating on.  A 16-bit crc may also be
excessive for a 16-bit data type.  No real impact to the code's
usefulness is expected by this change
</commit_message>
<xml_diff>
--- a/Test Matrix.xlsx
+++ b/Test Matrix.xlsx
@@ -160,20 +160,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,15 +476,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -520,22 +520,22 @@
         <v>1011</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>10</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4">
         <v>101</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2">
+      <c r="I3" s="4"/>
+      <c r="J3" s="4">
         <v>1</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4">
         <v>111</v>
       </c>
     </row>
@@ -550,20 +550,20 @@
         <v>10011</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="2">
+      <c r="E4" s="6"/>
+      <c r="F4" s="4">
         <v>1110</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4">
         <v>1001</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4">
         <v>1111</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2">
+      <c r="K4" s="4"/>
+      <c r="L4" s="4">
         <v>1101</v>
       </c>
     </row>
@@ -578,20 +578,20 @@
         <v>100101</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="2">
+      <c r="E5" s="6"/>
+      <c r="F5" s="4">
         <v>10000</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4">
         <v>11000</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4">
         <v>10101</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2">
+      <c r="K5" s="4"/>
+      <c r="L5" s="4">
         <v>0</v>
       </c>
     </row>
@@ -606,20 +606,20 @@
         <v>1100111</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="2">
+      <c r="E6" s="6"/>
+      <c r="F6" s="4">
         <v>1011</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
         <v>110</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2">
+      <c r="I6" s="4"/>
+      <c r="J6" s="4">
         <v>111</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
         <v>10011</v>
       </c>
     </row>
@@ -634,20 +634,20 @@
         <v>11001011</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="2">
+      <c r="E7" s="6"/>
+      <c r="F7" s="4">
         <v>11011</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4">
         <v>1001110</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2">
+      <c r="I7" s="4"/>
+      <c r="J7" s="4">
         <v>11101</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4">
         <v>1011000</v>
       </c>
     </row>
@@ -662,20 +662,20 @@
         <v>111001111</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="2">
+      <c r="E8" s="6"/>
+      <c r="F8" s="4">
         <v>10111100</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4">
         <v>10101110</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2">
+      <c r="I8" s="4"/>
+      <c r="J8" s="4">
         <v>11111110</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2">
+      <c r="K8" s="4"/>
+      <c r="L8" s="4">
         <v>10101110</v>
       </c>
     </row>
@@ -690,20 +690,20 @@
         <v>1000110011</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="2">
+      <c r="E9" s="6"/>
+      <c r="F9" s="4">
         <v>1001010</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4">
         <v>11</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2">
+      <c r="I9" s="4"/>
+      <c r="J9" s="4">
         <v>101111001</v>
       </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2">
+      <c r="K9" s="4"/>
+      <c r="L9" s="4">
         <v>101000000</v>
       </c>
     </row>
@@ -718,20 +718,20 @@
         <v>11001001111</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="2">
+      <c r="E10" s="6"/>
+      <c r="F10" s="4">
         <v>1110011000</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4">
         <v>101010100</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2">
+      <c r="I10" s="4"/>
+      <c r="J10" s="4">
         <v>111101001</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2">
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
         <v>1101110000</v>
       </c>
     </row>
@@ -746,20 +746,20 @@
         <v>101110110111</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="2">
+      <c r="E11" s="6"/>
+      <c r="F11" s="4">
         <v>101101000</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4">
         <v>1000010000</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2">
+      <c r="I11" s="4"/>
+      <c r="J11" s="4">
         <v>11011111111</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
         <v>11011010000</v>
       </c>
     </row>
@@ -774,20 +774,20 @@
         <v>1001100001111</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="2">
+      <c r="E12" s="6"/>
+      <c r="F12" s="4">
         <v>111011101011</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4">
         <v>1010110100</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2">
+      <c r="I12" s="4"/>
+      <c r="J12" s="4">
         <v>111000001000</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4">
         <v>100001100111</v>
       </c>
     </row>
@@ -802,20 +802,20 @@
         <v>11010101111111</v>
       </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6">
+      <c r="G13" s="8"/>
+      <c r="H13" s="8">
         <v>11110001010</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="2">
+      <c r="I13" s="8"/>
+      <c r="J13" s="4">
         <v>1101010100101</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="5"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -828,20 +828,20 @@
         <v>100111110011111</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="2">
+      <c r="E14" s="6"/>
+      <c r="F14" s="4">
         <v>111101001000</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="8">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4">
         <v>11001010100100</v>
       </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8">
+      <c r="I14" s="4"/>
+      <c r="J14" s="4">
         <v>1000110011</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="5"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -856,24 +856,24 @@
       <c r="D15" s="1">
         <v>1000111</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="2">
+      <c r="E15" s="6"/>
+      <c r="F15" s="4">
         <v>110010010</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="4">
         <v>100111</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="4">
         <v>1010110</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="4">
         <v>10001</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="4">
         <v>1101001101110</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="5"/>
+      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -888,26 +888,14 @@
       <c r="D16" s="1">
         <v>101011</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="2">
-        <v>1111001100</v>
-      </c>
-      <c r="G16" s="2">
-        <v>10110</v>
-      </c>
-      <c r="H16" s="2">
-        <v>10010010</v>
-      </c>
-      <c r="I16" s="2">
-        <v>11111011</v>
-      </c>
-      <c r="J16" s="2">
-        <v>1110011010</v>
-      </c>
-      <c r="K16" s="2">
-        <v>110101</v>
-      </c>
-      <c r="L16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -951,12 +939,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -991,7 +979,7 @@
       <c r="C3" s="1">
         <v>1011</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="2">
@@ -1017,7 +1005,7 @@
       <c r="C4" s="1">
         <v>10011</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="2">
         <v>1010</v>
       </c>
@@ -1041,7 +1029,7 @@
       <c r="C5" s="1">
         <v>100101</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="2">
         <v>0</v>
       </c>
@@ -1065,7 +1053,7 @@
       <c r="C6" s="1">
         <v>1100111</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="2">
         <v>110010</v>
       </c>
@@ -1089,7 +1077,7 @@
       <c r="C7" s="1">
         <v>11001011</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="2">
         <v>1001000</v>
       </c>
@@ -1113,7 +1101,7 @@
       <c r="C8" s="1">
         <v>111001111</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="2">
         <v>1101110</v>
       </c>
@@ -1137,7 +1125,7 @@
       <c r="C9" s="1">
         <v>1000110011</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="2">
         <v>101111101</v>
       </c>
@@ -1161,7 +1149,7 @@
       <c r="C10" s="1">
         <v>11001001111</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="2">
         <v>1100111001</v>
       </c>
@@ -1185,7 +1173,7 @@
       <c r="C11" s="1">
         <v>101110110111</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="2">
         <v>110001</v>
       </c>
@@ -1209,7 +1197,7 @@
       <c r="C12" s="1">
         <v>1001100001111</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="2">
         <v>100101111000</v>
       </c>
@@ -1233,7 +1221,7 @@
       <c r="C13" s="1">
         <v>11010101111111</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="2">
         <v>110011011000</v>
       </c>
@@ -1257,7 +1245,7 @@
       <c r="C14" s="1">
         <v>100111110011111</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="2">
         <v>101001000010</v>
       </c>
@@ -1281,7 +1269,7 @@
       <c r="C15" s="1">
         <v>1001111001000110</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="2">
         <v>1101111000000</v>
       </c>
@@ -1305,7 +1293,7 @@
       <c r="C16" s="1">
         <v>1.0001101100101E+16</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="2">
         <v>1110100001010000</v>
       </c>

</xml_diff>